<commit_message>
holerites e att ficha cadastral
</commit_message>
<xml_diff>
--- a/FICHA%20CADASTRAL%20-%20LOCATARIO%20(FISICA).xlsx
+++ b/FICHA%20CADASTRAL%20-%20LOCATARIO%20(FISICA).xlsx
@@ -1,11 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67E5836F-9890-9F47-B372-906CD8586BCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x224720\Documents\karencakes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="6465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -15,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Plan1!$A$1:$J$61</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>NOME COMPLETO</t>
   </si>
@@ -283,15 +287,84 @@
   <si>
     <t>* Enviar a ficha preenchida juntamente aos documentos solicitados diretamente ao e-mail do corretor responsável.</t>
   </si>
+  <si>
+    <t>41714197-x</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>Fernando Branbila Cunha Junior</t>
+  </si>
+  <si>
+    <t>13219-280</t>
+  </si>
+  <si>
+    <t>Rua Alfredo Vaz de Campos, 136</t>
+  </si>
+  <si>
+    <t>Jardim Tamoio</t>
+  </si>
+  <si>
+    <t>Jundiaí</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>(11)98563-3959</t>
+  </si>
+  <si>
+    <t>(11)99721-4932</t>
+  </si>
+  <si>
+    <t>fer_bcjr@hotmail.com</t>
+  </si>
+  <si>
+    <t>Brasileira</t>
+  </si>
+  <si>
+    <t>Solteiro</t>
+  </si>
+  <si>
+    <t>Intera Consultoria LTDA</t>
+  </si>
+  <si>
+    <t>(11)2691-4003</t>
+  </si>
+  <si>
+    <t>Analista Desenvolvedor Pleno</t>
+  </si>
+  <si>
+    <t>Karen Cristina Marques dos Santos</t>
+  </si>
+  <si>
+    <t>Rua Padre Norberto Mojola 274</t>
+  </si>
+  <si>
+    <t>13205-000</t>
+  </si>
+  <si>
+    <t>Jardim Santa Gertrudes</t>
+  </si>
+  <si>
+    <t>karen.marques36@gmail.com</t>
+  </si>
+  <si>
+    <t>Cristina</t>
+  </si>
+  <si>
+    <t>AP4290</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0##&quot;.&quot;###&quot;.&quot;###\-##"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +482,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -621,11 +708,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -756,6 +844,201 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -771,36 +1054,18 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,187 +1075,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="15" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1013,7 +1114,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1049,7 +1150,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1061,11 +1162,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2549,23 +2650,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2601,23 +2685,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2793,61 +2860,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J428"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.9609375" customWidth="1"/>
-    <col min="2" max="2" width="15.73828125" customWidth="1"/>
-    <col min="3" max="3" width="7.26171875" customWidth="1"/>
-    <col min="4" max="4" width="8.7421875" customWidth="1"/>
-    <col min="5" max="5" width="8.7421875" style="44" customWidth="1"/>
-    <col min="6" max="6" width="8.203125" style="44" customWidth="1"/>
-    <col min="7" max="7" width="7.80078125" customWidth="1"/>
-    <col min="8" max="8" width="6.1875" customWidth="1"/>
-    <col min="9" max="9" width="8.875" customWidth="1"/>
-    <col min="10" max="10" width="8.7421875" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="44" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="44" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="74"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="92"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="32" t="s">
+        <v>77</v>
+      </c>
       <c r="C2" s="33"/>
       <c r="D2" s="33"/>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
-      <c r="G2" s="110" t="s">
+      <c r="G2" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="111"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="58"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2" s="76"/>
+      <c r="I2" s="122" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="123"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2859,21 +2930,21 @@
       <c r="I3" s="18"/>
       <c r="J3" s="19"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="81" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="109" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="83"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="111"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -2885,21 +2956,21 @@
       <c r="I5" s="15"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="72" t="s">
+    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="74"/>
-    </row>
-    <row r="7" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="92"/>
+    </row>
+    <row r="7" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2911,119 +2982,119 @@
       <c r="I7" s="9"/>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="101" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="103"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="49"/>
-      <c r="F8" s="101" t="s">
+      <c r="F8" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="103"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="98" t="s">
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="95"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="87" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="99"/>
-      <c r="C9" s="100"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="3"/>
       <c r="E9" s="49"/>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="98" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="89"/>
       <c r="D10" s="3"/>
       <c r="E10" s="49"/>
-      <c r="F10" s="68" t="s">
+      <c r="F10" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="98" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="100"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="3"/>
       <c r="E11" s="49"/>
-      <c r="F11" s="68" t="s">
+      <c r="F11" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="98" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="100"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="3"/>
       <c r="E12" s="49"/>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="98" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="89"/>
       <c r="D13" s="3"/>
       <c r="E13" s="49"/>
-      <c r="F13" s="68" t="s">
+      <c r="F13" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="98" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="87" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="89"/>
       <c r="D14" s="3"/>
       <c r="E14" s="49"/>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -3035,236 +3106,274 @@
       <c r="I15" s="15"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="59" t="s">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="61"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="84"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="85"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="91"/>
-      <c r="C17" s="92"/>
+      <c r="B17" s="115">
+        <v>43241067890</v>
+      </c>
+      <c r="C17" s="116"/>
       <c r="D17" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="75"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="84" t="s">
+      <c r="E17" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="74"/>
+      <c r="G17" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="85"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="94"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H17" s="82"/>
+      <c r="I17" s="117" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17" s="118"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="77"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="73" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="108"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="80"/>
+      <c r="B19" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="100"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="100"/>
+      <c r="G19" s="100"/>
+      <c r="H19" s="99"/>
       <c r="I19" s="34" t="s">
         <v>33</v>
       </c>
       <c r="J19" s="38"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="38" t="s">
+        <v>58</v>
+      </c>
       <c r="C20" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="78"/>
-      <c r="E20" s="80"/>
+      <c r="D20" s="98" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="99"/>
       <c r="F20" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="106"/>
-      <c r="H20" s="107"/>
+      <c r="G20" s="101" t="s">
+        <v>61</v>
+      </c>
+      <c r="H20" s="102"/>
       <c r="I20" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="40"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J20" s="40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="80"/>
+      <c r="B21" s="98" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="99"/>
       <c r="F21" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="78"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79"/>
-      <c r="J21" s="80"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G21" s="98"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="99"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="80"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="131" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="100"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="99"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="84" t="s">
+      <c r="B23" s="98" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="100"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="85"/>
-      <c r="G23" s="88"/>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="90"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F23" s="82"/>
+      <c r="G23" s="112">
+        <v>34795</v>
+      </c>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="114"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="80"/>
+      <c r="B24" s="98" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="100"/>
+      <c r="D24" s="99"/>
       <c r="E24" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="78"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="80"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F24" s="98"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="99"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
       <c r="D25" s="42"/>
-      <c r="E25" s="123" t="s">
+      <c r="E25" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="124"/>
-      <c r="G25" s="124"/>
-      <c r="H25" s="125"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="67"/>
       <c r="I25" s="42"/>
       <c r="J25" s="43"/>
     </row>
-    <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="59" t="s">
+    <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="61"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="84"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="84"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="84"/>
+      <c r="G26" s="84"/>
+      <c r="H26" s="84"/>
+      <c r="I26" s="84"/>
+      <c r="J26" s="85"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="65"/>
+      <c r="B27" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="51" t="s">
         <v>36</v>
       </c>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
-      <c r="I27" s="26"/>
+      <c r="I27" s="26" t="s">
+        <v>69</v>
+      </c>
       <c r="J27" s="27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="97"/>
+      <c r="B28" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="63"/>
       <c r="D28" s="21"/>
       <c r="E28" s="50"/>
       <c r="F28" s="52"/>
-      <c r="G28" s="86"/>
-      <c r="H28" s="86"/>
-      <c r="I28" s="86"/>
-      <c r="J28" s="87"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G28" s="79"/>
+      <c r="H28" s="79"/>
+      <c r="I28" s="79"/>
+      <c r="J28" s="80"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="21"/>
+      <c r="B29" s="132">
+        <v>5000</v>
+      </c>
       <c r="C29" s="22"/>
-      <c r="D29" s="129" t="s">
+      <c r="D29" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="E29" s="130"/>
-      <c r="F29" s="50"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="134">
+        <v>1500</v>
+      </c>
       <c r="G29" s="22"/>
       <c r="H29" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="I29" s="22"/>
+      <c r="I29" s="133">
+        <v>6500</v>
+      </c>
       <c r="J29" s="4"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="97"/>
-      <c r="D30" s="97"/>
-      <c r="E30" s="65"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
       <c r="F30" s="51" t="s">
         <v>36</v>
       </c>
@@ -3273,30 +3382,30 @@
       <c r="I30" s="26"/>
       <c r="J30" s="27"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="97"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="63"/>
       <c r="D31" s="21"/>
       <c r="E31" s="50"/>
       <c r="F31" s="52"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="86"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="87"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="80"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="34" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="22"/>
-      <c r="D32" s="129" t="s">
+      <c r="D32" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="130"/>
+      <c r="E32" s="78"/>
       <c r="F32" s="50"/>
       <c r="G32" s="22"/>
       <c r="H32" s="28" t="s">
@@ -3305,227 +3414,255 @@
       <c r="I32" s="22"/>
       <c r="J32" s="4"/>
     </row>
-    <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="59" t="s">
+    <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="61"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B33" s="84"/>
+      <c r="C33" s="84"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="84"/>
+      <c r="J33" s="85"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="108"/>
-      <c r="C34" s="109"/>
+      <c r="B34" s="71">
+        <v>43784993800</v>
+      </c>
+      <c r="C34" s="72"/>
       <c r="D34" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="75"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="84" t="s">
+      <c r="E34" s="73">
+        <v>495653871</v>
+      </c>
+      <c r="F34" s="74"/>
+      <c r="G34" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H34" s="85"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="96"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H34" s="82"/>
+      <c r="I34" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="J34" s="61"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="69"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="71"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="128" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="129"/>
+      <c r="D35" s="129"/>
+      <c r="E35" s="129"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="129"/>
+      <c r="H35" s="129"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="130"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="97"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="65"/>
+      <c r="B36" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="64"/>
       <c r="I36" s="34" t="s">
         <v>33</v>
       </c>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="13"/>
+      <c r="B37" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="C37" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="65"/>
+      <c r="D37" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="64"/>
       <c r="F37" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G37" s="104"/>
-      <c r="H37" s="105"/>
+      <c r="G37" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="97"/>
       <c r="I37" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J37" s="4"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J37" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="64"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="64"/>
-      <c r="E38" s="65"/>
+      <c r="B38" s="98" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="99"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G38" s="64"/>
-      <c r="H38" s="97"/>
-      <c r="I38" s="97"/>
-      <c r="J38" s="65"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G38" s="62"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="64"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="64"/>
-      <c r="C39" s="97"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="97"/>
-      <c r="G39" s="97"/>
-      <c r="H39" s="97"/>
-      <c r="I39" s="97"/>
-      <c r="J39" s="65"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B39" s="131" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="63"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63"/>
+      <c r="H39" s="63"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="64"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="64"/>
-      <c r="C40" s="97"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="84" t="s">
+      <c r="B40" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="63"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="85"/>
-      <c r="G40" s="112"/>
-      <c r="H40" s="113"/>
-      <c r="I40" s="113"/>
-      <c r="J40" s="114"/>
-    </row>
-    <row r="41" spans="1:10" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="59" t="s">
+      <c r="F40" s="82"/>
+      <c r="G40" s="103">
+        <v>35071</v>
+      </c>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="105"/>
+    </row>
+    <row r="41" spans="1:10" s="30" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="60"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="60"/>
-      <c r="J41" s="61"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="84"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="85"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
         <v>24</v>
       </c>
       <c r="B42" s="12"/>
-      <c r="C42" s="115" t="s">
+      <c r="C42" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="116"/>
+      <c r="D42" s="107"/>
       <c r="E42" s="42"/>
       <c r="F42" s="42"/>
-      <c r="G42" s="66" t="s">
+      <c r="G42" s="126" t="s">
         <v>14</v>
       </c>
-      <c r="H42" s="67"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="63"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="54" t="s">
+      <c r="H42" s="127"/>
+      <c r="I42" s="124"/>
+      <c r="J42" s="125"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="55"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="70"/>
-      <c r="F43" s="70"/>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="71"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="54" t="s">
+      <c r="B43" s="120"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="128"/>
+      <c r="E43" s="129"/>
+      <c r="F43" s="129"/>
+      <c r="G43" s="129"/>
+      <c r="H43" s="129"/>
+      <c r="I43" s="129"/>
+      <c r="J43" s="130"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="97"/>
-      <c r="F44" s="97"/>
-      <c r="G44" s="97"/>
-      <c r="H44" s="97"/>
-      <c r="I44" s="97"/>
-      <c r="J44" s="65"/>
-    </row>
-    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="59" t="s">
+      <c r="B44" s="120"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="62">
+        <v>2</v>
+      </c>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="64"/>
+    </row>
+    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="60"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="60"/>
-      <c r="G45" s="60"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="60"/>
-      <c r="J45" s="61"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="84"/>
+      <c r="C45" s="84"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84"/>
+      <c r="F45" s="84"/>
+      <c r="G45" s="84"/>
+      <c r="H45" s="84"/>
+      <c r="I45" s="84"/>
+      <c r="J45" s="85"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B46" s="108"/>
-      <c r="C46" s="109"/>
+      <c r="B46" s="71"/>
+      <c r="C46" s="72"/>
       <c r="D46" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="75"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="110" t="s">
+      <c r="E46" s="73"/>
+      <c r="F46" s="74"/>
+      <c r="G46" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="H46" s="111"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="96"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H46" s="76"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="61"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>0</v>
       </c>
@@ -3538,40 +3675,40 @@
         <v>44</v>
       </c>
       <c r="H47" s="25"/>
-      <c r="I47" s="95"/>
-      <c r="J47" s="96"/>
-    </row>
-    <row r="48" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="126"/>
-      <c r="B48" s="127"/>
-      <c r="C48" s="127"/>
-      <c r="D48" s="127"/>
-      <c r="E48" s="127"/>
-      <c r="F48" s="127"/>
-      <c r="G48" s="127"/>
-      <c r="H48" s="127"/>
-      <c r="I48" s="127"/>
-      <c r="J48" s="128"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I47" s="60"/>
+      <c r="J47" s="61"/>
+    </row>
+    <row r="48" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="68"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="70"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B49" s="108"/>
-      <c r="C49" s="109"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="72"/>
       <c r="D49" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E49" s="75"/>
-      <c r="F49" s="76"/>
-      <c r="G49" s="110" t="s">
+      <c r="E49" s="73"/>
+      <c r="F49" s="74"/>
+      <c r="G49" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="H49" s="111"/>
-      <c r="I49" s="95"/>
-      <c r="J49" s="96"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H49" s="76"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="61"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>0</v>
       </c>
@@ -3584,40 +3721,40 @@
         <v>44</v>
       </c>
       <c r="H50" s="25"/>
-      <c r="I50" s="95"/>
-      <c r="J50" s="96"/>
-    </row>
-    <row r="51" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="126"/>
-      <c r="B51" s="127"/>
-      <c r="C51" s="127"/>
-      <c r="D51" s="127"/>
-      <c r="E51" s="127"/>
-      <c r="F51" s="127"/>
-      <c r="G51" s="127"/>
-      <c r="H51" s="127"/>
-      <c r="I51" s="127"/>
-      <c r="J51" s="128"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I50" s="60"/>
+      <c r="J50" s="61"/>
+    </row>
+    <row r="51" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="68"/>
+      <c r="B51" s="69"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
+      <c r="J51" s="70"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="108"/>
-      <c r="C52" s="109"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="72"/>
       <c r="D52" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E52" s="75"/>
-      <c r="F52" s="76"/>
-      <c r="G52" s="110" t="s">
+      <c r="E52" s="73"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="H52" s="111"/>
-      <c r="I52" s="95"/>
-      <c r="J52" s="96"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H52" s="76"/>
+      <c r="I52" s="60"/>
+      <c r="J52" s="61"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
         <v>0</v>
       </c>
@@ -3630,40 +3767,40 @@
         <v>44</v>
       </c>
       <c r="H53" s="23"/>
-      <c r="I53" s="95"/>
-      <c r="J53" s="96"/>
-    </row>
-    <row r="54" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="126"/>
-      <c r="B54" s="127"/>
-      <c r="C54" s="127"/>
-      <c r="D54" s="127"/>
-      <c r="E54" s="127"/>
-      <c r="F54" s="127"/>
-      <c r="G54" s="127"/>
-      <c r="H54" s="127"/>
-      <c r="I54" s="127"/>
-      <c r="J54" s="128"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I53" s="60"/>
+      <c r="J53" s="61"/>
+    </row>
+    <row r="54" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="68"/>
+      <c r="B54" s="69"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
+      <c r="I54" s="69"/>
+      <c r="J54" s="70"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="108"/>
-      <c r="C55" s="109"/>
+      <c r="B55" s="71"/>
+      <c r="C55" s="72"/>
       <c r="D55" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E55" s="75"/>
-      <c r="F55" s="76"/>
-      <c r="G55" s="110" t="s">
+      <c r="E55" s="73"/>
+      <c r="F55" s="74"/>
+      <c r="G55" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="H55" s="111"/>
-      <c r="I55" s="95"/>
-      <c r="J55" s="96"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H55" s="76"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="61"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>0</v>
       </c>
@@ -3676,40 +3813,40 @@
         <v>44</v>
       </c>
       <c r="H56" s="25"/>
-      <c r="I56" s="95"/>
-      <c r="J56" s="96"/>
-    </row>
-    <row r="57" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="126"/>
-      <c r="B57" s="127"/>
-      <c r="C57" s="127"/>
-      <c r="D57" s="127"/>
-      <c r="E57" s="127"/>
-      <c r="F57" s="127"/>
-      <c r="G57" s="127"/>
-      <c r="H57" s="127"/>
-      <c r="I57" s="127"/>
-      <c r="J57" s="128"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I56" s="60"/>
+      <c r="J56" s="61"/>
+    </row>
+    <row r="57" spans="1:10" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="68"/>
+      <c r="B57" s="69"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="69"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="69"/>
+      <c r="I57" s="69"/>
+      <c r="J57" s="70"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="108"/>
-      <c r="C58" s="109"/>
+      <c r="B58" s="71"/>
+      <c r="C58" s="72"/>
       <c r="D58" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E58" s="75"/>
-      <c r="F58" s="76"/>
-      <c r="G58" s="110" t="s">
+      <c r="E58" s="73"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="H58" s="111"/>
-      <c r="I58" s="95"/>
-      <c r="J58" s="96"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H58" s="76"/>
+      <c r="I58" s="60"/>
+      <c r="J58" s="61"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
         <v>0</v>
       </c>
@@ -3722,36 +3859,36 @@
         <v>44</v>
       </c>
       <c r="H59" s="23"/>
-      <c r="I59" s="95"/>
-      <c r="J59" s="96"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="117" t="s">
+      <c r="I59" s="60"/>
+      <c r="J59" s="61"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B60" s="118"/>
-      <c r="C60" s="118"/>
-      <c r="D60" s="118"/>
-      <c r="E60" s="118"/>
-      <c r="F60" s="118"/>
-      <c r="G60" s="118"/>
-      <c r="H60" s="118"/>
-      <c r="I60" s="118"/>
-      <c r="J60" s="119"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="120"/>
-      <c r="B61" s="121"/>
-      <c r="C61" s="121"/>
-      <c r="D61" s="121"/>
-      <c r="E61" s="121"/>
-      <c r="F61" s="121"/>
-      <c r="G61" s="121"/>
-      <c r="H61" s="121"/>
-      <c r="I61" s="121"/>
-      <c r="J61" s="122"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="55"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
+      <c r="G60" s="55"/>
+      <c r="H60" s="55"/>
+      <c r="I60" s="55"/>
+      <c r="J60" s="56"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="57"/>
+      <c r="B61" s="58"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="58"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="58"/>
+      <c r="J61" s="59"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="1"/>
@@ -3763,1472 +3900,1549 @@
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
       <c r="B265" s="2"/>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
       <c r="B266" s="2"/>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
       <c r="B267" s="2"/>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
       <c r="B268" s="2"/>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
       <c r="B269" s="2"/>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
       <c r="B270" s="2"/>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
       <c r="B271" s="2"/>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
       <c r="B273" s="2"/>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
       <c r="B275" s="2"/>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="2"/>
       <c r="B278" s="2"/>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="2"/>
       <c r="B279" s="2"/>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="2"/>
       <c r="B280" s="2"/>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="2"/>
       <c r="B283" s="2"/>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="2"/>
       <c r="B285" s="2"/>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="2"/>
       <c r="B286" s="2"/>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="2"/>
       <c r="B287" s="2"/>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="2"/>
       <c r="B296" s="2"/>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="2"/>
       <c r="B297" s="2"/>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="2"/>
       <c r="B298" s="2"/>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="2"/>
       <c r="B299" s="2"/>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="2"/>
       <c r="B300" s="2"/>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="2"/>
       <c r="B301" s="2"/>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" s="2"/>
       <c r="B302" s="2"/>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" s="2"/>
       <c r="B303" s="2"/>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
       <c r="B304" s="2"/>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" s="2"/>
       <c r="B305" s="2"/>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" s="2"/>
       <c r="B306" s="2"/>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" s="2"/>
       <c r="B307" s="2"/>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" s="2"/>
       <c r="B308" s="2"/>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" s="2"/>
       <c r="B309" s="2"/>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" s="2"/>
       <c r="B310" s="2"/>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" s="2"/>
       <c r="B311" s="2"/>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" s="2"/>
       <c r="B312" s="2"/>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" s="2"/>
       <c r="B313" s="2"/>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" s="2"/>
       <c r="B314" s="2"/>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" s="2"/>
       <c r="B315" s="2"/>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" s="2"/>
       <c r="B316" s="2"/>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" s="2"/>
       <c r="B317" s="2"/>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" s="2"/>
       <c r="B318" s="2"/>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" s="2"/>
       <c r="B319" s="2"/>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" s="2"/>
       <c r="B320" s="2"/>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" s="2"/>
       <c r="B321" s="2"/>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" s="2"/>
       <c r="B322" s="2"/>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" s="2"/>
       <c r="B323" s="2"/>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" s="2"/>
       <c r="B324" s="2"/>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" s="2"/>
       <c r="B325" s="2"/>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" s="2"/>
       <c r="B326" s="2"/>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" s="2"/>
       <c r="B327" s="2"/>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" s="2"/>
       <c r="B328" s="2"/>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" s="2"/>
       <c r="B329" s="2"/>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" s="2"/>
       <c r="B330" s="2"/>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" s="2"/>
       <c r="B331" s="2"/>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" s="2"/>
       <c r="B332" s="2"/>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" s="2"/>
       <c r="B333" s="2"/>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" s="2"/>
       <c r="B334" s="2"/>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" s="2"/>
       <c r="B335" s="2"/>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" s="2"/>
       <c r="B336" s="2"/>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" s="2"/>
       <c r="B337" s="2"/>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" s="2"/>
       <c r="B338" s="2"/>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" s="2"/>
       <c r="B339" s="2"/>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" s="2"/>
       <c r="B340" s="2"/>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" s="2"/>
       <c r="B341" s="2"/>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" s="2"/>
       <c r="B342" s="2"/>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" s="2"/>
       <c r="B343" s="2"/>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" s="2"/>
       <c r="B344" s="2"/>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" s="2"/>
       <c r="B345" s="2"/>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" s="2"/>
       <c r="B346" s="2"/>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" s="2"/>
       <c r="B347" s="2"/>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" s="2"/>
       <c r="B348" s="2"/>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" s="2"/>
       <c r="B349" s="2"/>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" s="2"/>
       <c r="B350" s="2"/>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" s="2"/>
       <c r="B351" s="2"/>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" s="2"/>
       <c r="B352" s="2"/>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" s="2"/>
       <c r="B353" s="2"/>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" s="2"/>
       <c r="B354" s="2"/>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" s="2"/>
       <c r="B355" s="2"/>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" s="2"/>
       <c r="B356" s="2"/>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" s="2"/>
       <c r="B357" s="2"/>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" s="2"/>
       <c r="B358" s="2"/>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" s="2"/>
       <c r="B359" s="2"/>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" s="2"/>
       <c r="B360" s="2"/>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" s="2"/>
       <c r="B361" s="2"/>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" s="2"/>
       <c r="B362" s="2"/>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" s="2"/>
       <c r="B363" s="2"/>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" s="2"/>
       <c r="B364" s="2"/>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" s="2"/>
       <c r="B365" s="2"/>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" s="2"/>
       <c r="B366" s="2"/>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" s="2"/>
       <c r="B367" s="2"/>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" s="2"/>
       <c r="B368" s="2"/>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" s="2"/>
       <c r="B369" s="2"/>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" s="2"/>
       <c r="B370" s="2"/>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" s="2"/>
       <c r="B371" s="2"/>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" s="2"/>
       <c r="B372" s="2"/>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" s="2"/>
       <c r="B373" s="2"/>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" s="2"/>
       <c r="B374" s="2"/>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" s="2"/>
       <c r="B375" s="2"/>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" s="2"/>
       <c r="B376" s="2"/>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" s="2"/>
       <c r="B377" s="2"/>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" s="2"/>
       <c r="B378" s="2"/>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" s="2"/>
       <c r="B379" s="2"/>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" s="2"/>
       <c r="B380" s="2"/>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" s="2"/>
       <c r="B381" s="2"/>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" s="2"/>
       <c r="B382" s="2"/>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" s="2"/>
       <c r="B383" s="2"/>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" s="2"/>
       <c r="B384" s="2"/>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" s="2"/>
       <c r="B385" s="2"/>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" s="2"/>
       <c r="B386" s="2"/>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" s="2"/>
       <c r="B387" s="2"/>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" s="2"/>
       <c r="B388" s="2"/>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" s="2"/>
       <c r="B389" s="2"/>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" s="2"/>
       <c r="B390" s="2"/>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" s="2"/>
       <c r="B391" s="2"/>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" s="2"/>
       <c r="B392" s="2"/>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" s="2"/>
       <c r="B393" s="2"/>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" s="2"/>
       <c r="B394" s="2"/>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" s="2"/>
       <c r="B395" s="2"/>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" s="2"/>
       <c r="B396" s="2"/>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" s="2"/>
       <c r="B397" s="2"/>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" s="2"/>
       <c r="B398" s="2"/>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" s="2"/>
       <c r="B399" s="2"/>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" s="2"/>
       <c r="B400" s="2"/>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" s="2"/>
       <c r="B401" s="2"/>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A402" s="2"/>
       <c r="B402" s="2"/>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A403" s="2"/>
       <c r="B403" s="2"/>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A404" s="2"/>
       <c r="B404" s="2"/>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A405" s="2"/>
       <c r="B405" s="2"/>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A406" s="2"/>
       <c r="B406" s="2"/>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A407" s="2"/>
       <c r="B407" s="2"/>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A408" s="2"/>
       <c r="B408" s="2"/>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A409" s="2"/>
       <c r="B409" s="2"/>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A410" s="2"/>
       <c r="B410" s="2"/>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A411" s="2"/>
       <c r="B411" s="2"/>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A412" s="2"/>
       <c r="B412" s="2"/>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A413" s="2"/>
       <c r="B413" s="2"/>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A414" s="2"/>
       <c r="B414" s="2"/>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A415" s="2"/>
       <c r="B415" s="2"/>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A416" s="2"/>
       <c r="B416" s="2"/>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A417" s="2"/>
       <c r="B417" s="2"/>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A418" s="2"/>
       <c r="B418" s="2"/>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A419" s="2"/>
       <c r="B419" s="2"/>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A420" s="2"/>
       <c r="B420" s="2"/>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A421" s="2"/>
       <c r="B421" s="2"/>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A422" s="2"/>
       <c r="B422" s="2"/>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A423" s="2"/>
       <c r="B423" s="2"/>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A424" s="2"/>
       <c r="B424" s="2"/>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A425" s="2"/>
       <c r="B425" s="2"/>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A426" s="2"/>
       <c r="B426" s="2"/>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A427" s="2"/>
       <c r="B427" s="2"/>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A428" s="2"/>
       <c r="B428" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="102">
+  <mergeCells count="101">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="B18:J18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:J24"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
     <mergeCell ref="A60:J61"/>
     <mergeCell ref="I59:J59"/>
     <mergeCell ref="B27:E27"/>
@@ -5253,95 +5467,21 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="G34:H34"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="B18:J18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F12:I12"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="B35:J35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D44:J44"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1"/>
+    <hyperlink ref="B39" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Check Box 1">
+            <control shapeId="1025" r:id="rId6" name="Check Box 1">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5363,7 +5503,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+            <control shapeId="1026" r:id="rId7" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5385,7 +5525,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1029" r:id="rId6" name="Check Box 5">
+            <control shapeId="1029" r:id="rId8" name="Check Box 5">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5407,7 +5547,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1030" r:id="rId7" name="Check Box 6">
+            <control shapeId="1030" r:id="rId9" name="Check Box 6">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5429,7 +5569,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId8" name="Check Box 15">
+            <control shapeId="1039" r:id="rId10" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5451,7 +5591,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId9" name="Check Box 16">
+            <control shapeId="1040" r:id="rId11" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5473,7 +5613,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId10" name="Check Box 17">
+            <control shapeId="1041" r:id="rId12" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5495,7 +5635,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId11" name="Check Box 18">
+            <control shapeId="1042" r:id="rId13" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5517,7 +5657,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId12" name="Check Box 19">
+            <control shapeId="1043" r:id="rId14" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5539,7 +5679,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId13" name="Check Box 20">
+            <control shapeId="1044" r:id="rId15" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5561,7 +5701,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId14" name="Check Box 21">
+            <control shapeId="1045" r:id="rId16" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5583,7 +5723,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId15" name="Check Box 22">
+            <control shapeId="1046" r:id="rId17" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5605,7 +5745,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId16" name="Check Box 23">
+            <control shapeId="1047" r:id="rId18" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5627,7 +5767,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId17" name="Check Box 24">
+            <control shapeId="1048" r:id="rId19" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5649,7 +5789,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId18" name="Check Box 25">
+            <control shapeId="1049" r:id="rId20" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5671,7 +5811,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId19" name="Check Box 26">
+            <control shapeId="1050" r:id="rId21" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -5698,24 +5838,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>